<commit_message>
Complete chages required by new UI design added
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/fileTemplates/HolidaysTemplate.xlsx
+++ b/src/main/resources/templates/fileTemplates/HolidaysTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\waaw\waaw-backend\src\main\resources\templates\fileTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -38,9 +38,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>Christmas</t>
   </si>
   <si>
@@ -51,6 +48,9 @@
   </si>
   <si>
     <t>Founder's Day</t>
+  </si>
+  <si>
+    <t>holiday_type</t>
   </si>
 </sst>
 </file>
@@ -371,7 +371,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,12 +397,12 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>2022</v>
@@ -414,12 +414,12 @@
         <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>2022</v>
@@ -431,7 +431,7 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>